<commit_message>
Updated kNN and Naive Bayes slides and examples. Plus draft regression slides and examples
</commit_message>
<xml_diff>
--- a/slides/KNN.xlsx
+++ b/slides/KNN.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_cmps460-content\slides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF287F4-BE89-4A35-89B6-2AFCEE915E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BCF75E-EA32-46A6-A045-838BBAB14581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="knn" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>M</t>
   </si>
@@ -63,20 +62,23 @@
     <t>L</t>
   </si>
   <si>
-    <t>Height (in cms)</t>
+    <t>Ali walks in to the shop</t>
   </si>
   <si>
-    <t>Weight (in kgs)</t>
+    <t>His weight (Kg)</t>
   </si>
   <si>
-    <t>T Shirt Size</t>
+    <t>His height (cm)</t>
+  </si>
+  <si>
+    <t>Recommend a shirt size?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,19 +94,36 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF111111"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,19 +143,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6A798B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF9FAFB"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -150,17 +157,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF54585D"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color rgb="FF54585D"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color rgb="FF54585D"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF54585D"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -169,36 +176,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -245,8 +283,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Data</a:t>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Shirt size based on Weight and Height</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -290,7 +328,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Datos</c:v>
+            <c:v>Shirt size based on Weight and Height</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -304,7 +342,7 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
@@ -322,8 +360,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{477FC6A2-43F2-4113-9E41-D5CC5820A2A9}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{E41C1C99-4B45-478E-9BBC-2248D74474C3}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -355,8 +393,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{38267FE5-DDAE-4053-B106-18D2F034D629}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{6E49AA84-4094-4476-9CB4-507C967FC094}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -388,8 +426,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{600B41AF-6549-4698-9ACF-17DF0BCB87E6}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{B28C2191-88BF-4A2B-8B9C-50851EB1175D}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -421,8 +459,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{730854A8-1C0F-41C6-88FE-563D1AA6EA2F}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{17E3C056-3094-444A-814C-020389AC555E}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -454,8 +492,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{563DB685-A99F-4ADB-9FF1-8A6ECA40CF33}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{0C3BDAED-A87D-408E-A331-BAA404FC7332}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -487,8 +525,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B0DD04AC-6984-431D-A4B3-765D5FA1F698}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{52F327A4-9B5E-4A0B-A57F-1E35EB265450}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -520,8 +558,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D36F15A-5782-43BF-8224-F0ECFAD9D22E}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{A3EB4374-5C14-4D6F-9BED-0DA5108F156C}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -553,8 +591,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B2E0154E-BE60-42C7-B196-7F45B828CF1E}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{84757474-3E9A-4B14-86C6-3918040FD8CD}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -586,8 +624,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A581C450-5576-4D09-9135-F55FF20C0D21}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{935A997D-E8A3-445E-B497-89AD201D0BDA}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -619,8 +657,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3B3FA4AA-1E1B-45EC-8906-FA40EB956F81}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{B0D922C1-0F14-4D83-A77D-E2E381F66B44}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -704,7 +742,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>knn!$A$7:$A$16</c:f>
+              <c:f>knn!$A$6:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -743,7 +781,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>knn!$B$7:$B$16</c:f>
+              <c:f>knn!$B$6:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -784,7 +822,7 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>knn!$C$7:$C$16</c15:f>
+                <c15:f>knn!$C$6:$C$15</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="10"/>
                   <c:pt idx="0">
@@ -846,7 +884,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>knn!$C$6</c15:sqref>
+                          <c15:sqref>knn!$C$5</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -885,7 +923,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>knn!$A$7:$A$16</c15:sqref>
+                          <c15:sqref>knn!$A$6:$A$15</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -930,7 +968,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>knn!$C$7:$C$16</c15:sqref>
+                          <c15:sqref>knn!$C$6:$C$15</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1003,6 +1041,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Weight</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1065,6 +1158,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Height</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1712,15 +1860,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>361949</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>254001</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2011,481 +2159,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.1796875" customWidth="1"/>
     <col min="3" max="3" width="14.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2">
+        <v>76</v>
+      </c>
+    </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C2" s="1" t="s">
-        <v>4</v>
+      <c r="C2" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="D2" s="2">
         <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C3" s="1" t="s">
+      <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f>INDEX($C$5:$E$15,MATCH(1,E5:E15,0),1)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="str">
-        <f>INDEX($C$6:$E$16,MATCH(1,E6:E16,0),1)</f>
-        <v>M</v>
+      <c r="D5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1</v>
+      <c r="A6" s="3">
+        <v>55</v>
+      </c>
+      <c r="B6" s="3">
+        <v>160</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5">
+        <f>SQRT(($D$2-B6)^2 + ($D$1-A6)^2)</f>
+        <v>23.259406699226016</v>
+      </c>
+      <c r="E6" s="3">
+        <f>RANK(D6,$D$6:$D$15,1)</f>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>55</v>
-      </c>
-      <c r="B7">
-        <v>160</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="A7" s="3">
+        <v>58</v>
+      </c>
+      <c r="B7" s="3">
+        <v>165</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="3">
-        <f>SQRT(($D$2-B7)^2 + ($D$3-A7)^2)</f>
-        <v>17.204650534085253</v>
-      </c>
-      <c r="E7">
-        <f>RANK(D7,$D$7:$D$16,1)</f>
-        <v>8</v>
+      <c r="D7" s="5">
+        <f>SQRT(($D$2-B7)^2 + ($D$1-A7)^2)</f>
+        <v>18.681541692269406</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" ref="E7:E15" si="0">RANK(D7,$D$6:$D$15,1)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>58</v>
-      </c>
-      <c r="B8">
-        <v>165</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="3">
-        <f t="shared" ref="D8:D16" si="0">SQRT(($D$2-B8)^2 + ($D$3-A8)^2)</f>
-        <v>12.083045973594572</v>
-      </c>
-      <c r="E8">
-        <f t="shared" ref="E8:E16" si="1">RANK(D8,$D$7:$D$16,1)</f>
-        <v>6</v>
+      <c r="A8" s="3">
+        <v>60</v>
+      </c>
+      <c r="B8" s="3">
+        <v>160</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <f>SQRT(($D$2-B8)^2 + ($D$1-A8)^2)</f>
+        <v>18.867962264113206</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>60</v>
-      </c>
-      <c r="B9">
-        <v>160</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="A9" s="11">
+        <v>65</v>
+      </c>
+      <c r="B9" s="11">
+        <v>166</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="13">
+        <f>SQRT(($D$2-B9)^2 + ($D$1-A9)^2)</f>
+        <v>11.704699910719626</v>
+      </c>
+      <c r="E9" s="14">
         <f t="shared" si="0"/>
-        <v>13.45362404707371</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
-        <v>65</v>
-      </c>
-      <c r="B10" s="4">
-        <v>166</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="A10" s="11">
+        <v>70</v>
+      </c>
+      <c r="B10" s="11">
+        <v>168</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="13">
+        <f>SQRT(($D$2-B10)^2 + ($D$1-A10)^2)</f>
+        <v>6.324555320336759</v>
+      </c>
+      <c r="E10" s="14">
         <f t="shared" si="0"/>
-        <v>5.6568542494923806</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
-        <v>70</v>
-      </c>
-      <c r="B11" s="4">
-        <v>168</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="A11" s="11">
+        <v>68</v>
+      </c>
+      <c r="B11" s="11">
+        <v>171</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="13">
+        <f>SQRT(($D$2-B11)^2 + ($D$1-A11)^2)</f>
+        <v>8.0622577482985491</v>
+      </c>
+      <c r="E11" s="14">
         <f t="shared" si="0"/>
-        <v>2.2360679774997898</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
-        <v>68</v>
-      </c>
-      <c r="B12" s="4">
-        <v>171</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
+      <c r="A12" s="3">
+        <v>75</v>
+      </c>
+      <c r="B12" s="3">
+        <v>175</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="5">
+        <f>SQRT(($D$2-B12)^2 + ($D$1-A12)^2)</f>
+        <v>5.0990195135927845</v>
+      </c>
+      <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>75</v>
       </c>
-      <c r="B13">
-        <v>175</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="3">
+        <v>180</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="5">
+        <f>SQRT(($D$2-B13)^2 + ($D$1-A13)^2)</f>
+        <v>10.04987562112089</v>
+      </c>
+      <c r="E13" s="3">
         <f t="shared" si="0"/>
-        <v>7.810249675906654</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>75</v>
-      </c>
-      <c r="B14">
-        <v>180</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="A14" s="3">
+        <v>80</v>
+      </c>
+      <c r="B14" s="3">
+        <v>187</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="5">
+        <f>SQRT(($D$2-B14)^2 + ($D$1-A14)^2)</f>
+        <v>17.464249196572979</v>
+      </c>
+      <c r="E14" s="3">
         <f t="shared" si="0"/>
-        <v>11.661903789690601</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>80</v>
-      </c>
-      <c r="B15">
-        <v>187</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="A15" s="3">
+        <v>90</v>
+      </c>
+      <c r="B15" s="3">
+        <v>190</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="5">
+        <f>SQRT(($D$2-B15)^2 + ($D$1-A15)^2)</f>
+        <v>24.413111231467404</v>
+      </c>
+      <c r="E15" s="3">
         <f t="shared" si="0"/>
-        <v>20.248456731316587</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>90</v>
-      </c>
-      <c r="B16">
-        <v>190</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="3">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E6:E15">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:E15">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$E6 &lt;= 3</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02F04BEC-B5BB-4736-A11F-40E400A234DC}">
-  <dimension ref="A1:C19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.7265625" customWidth="1"/>
-    <col min="2" max="2" width="9.90625" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="47" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="9">
-        <v>158</v>
-      </c>
-      <c r="B2" s="9">
-        <v>58</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="10">
-        <v>158</v>
-      </c>
-      <c r="B3" s="10">
-        <v>59</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="9">
-        <v>158</v>
-      </c>
-      <c r="B4" s="9">
-        <v>63</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="10">
-        <v>160</v>
-      </c>
-      <c r="B5" s="10">
-        <v>59</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="9">
-        <v>160</v>
-      </c>
-      <c r="B6" s="9">
-        <v>60</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="10">
-        <v>163</v>
-      </c>
-      <c r="B7" s="10">
-        <v>60</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="9">
-        <v>163</v>
-      </c>
-      <c r="B8" s="9">
-        <v>61</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="10">
-        <v>160</v>
-      </c>
-      <c r="B9" s="10">
-        <v>64</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="9">
-        <v>163</v>
-      </c>
-      <c r="B10" s="9">
-        <v>64</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="10">
-        <v>165</v>
-      </c>
-      <c r="B11" s="10">
-        <v>61</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="9">
-        <v>165</v>
-      </c>
-      <c r="B12" s="9">
-        <v>62</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="10">
-        <v>165</v>
-      </c>
-      <c r="B13" s="10">
-        <v>65</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="9">
-        <v>168</v>
-      </c>
-      <c r="B14" s="9">
-        <v>62</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="10">
-        <v>168</v>
-      </c>
-      <c r="B15" s="10">
-        <v>63</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="9">
-        <v>168</v>
-      </c>
-      <c r="B16" s="9">
-        <v>66</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="10">
-        <v>170</v>
-      </c>
-      <c r="B17" s="10">
-        <v>63</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="9">
-        <v>170</v>
-      </c>
-      <c r="B18" s="9">
-        <v>64</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="10">
-        <v>170</v>
-      </c>
-      <c r="B19" s="10">
-        <v>68</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>